<commit_message>
Actualizacion del plan general
</commit_message>
<xml_diff>
--- a/tspi/ciclo-4/plan4-20106381.xlsx
+++ b/tspi/ciclo-4/plan4-20106381.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="819" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="819" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="45">
   <si>
     <t>Id</t>
   </si>
@@ -136,9 +136,6 @@
     <t>Comentario</t>
   </si>
   <si>
-    <t>10/13/2014</t>
-  </si>
-  <si>
     <t>Reporte de pm y peer review form. Ciclo #3</t>
   </si>
   <si>
@@ -155,6 +152,9 @@
   </si>
   <si>
     <t>Version Final del documento de calidad</t>
+  </si>
+  <si>
+    <t>Testeo Funcionalidad #4</t>
   </si>
 </sst>
 </file>
@@ -785,8 +785,8 @@
   </sheetPr>
   <dimension ref="1:10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3954,7 +3954,30 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7" t="n">
+        <v>75</v>
+      </c>
+      <c r="B9" s="7" t="n">
+        <f aca="false">SUMIF(logt!G9:G16,A9,logt!F9:F16)/60</f>
+        <v>2</v>
+      </c>
+      <c r="C9" s="3" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="7" t="n">
+        <v>78</v>
+      </c>
+      <c r="B10" s="7" t="n">
+        <f aca="false">SUMIF(logt!G10:G17,A10,logt!F10:F17)/60</f>
+        <v>0.716666666666667</v>
+      </c>
+      <c r="C10" s="3" t="n">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -3971,10 +3994,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:9"/>
+  <dimension ref="1:11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4013,7 +4036,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="13" t="n">
-        <v>41924</v>
+        <v>41955</v>
       </c>
       <c r="B2" s="7" t="n">
         <v>8</v>
@@ -5053,8 +5076,8 @@
       <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="13" t="s">
-        <v>38</v>
+      <c r="A3" s="13" t="n">
+        <v>41956</v>
       </c>
       <c r="B3" s="7" t="n">
         <v>8</v>
@@ -6097,7 +6120,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="13" t="n">
-        <v>41930</v>
+        <v>41961</v>
       </c>
       <c r="B4" s="7" t="n">
         <v>9</v>
@@ -6119,7 +6142,7 @@
         <v>61</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I4" s="0"/>
       <c r="J4" s="0"/>
@@ -7151,6 +7174,7 @@
       <c r="D5" s="14" t="n">
         <v>0.409722222222222</v>
       </c>
+      <c r="E5" s="0"/>
       <c r="F5" s="15" t="n">
         <f aca="false">((HOUR(D5)-HOUR(C5))*60)+(MINUTE(D5)-MINUTE(C5))-E5</f>
         <v>110</v>
@@ -7159,7 +7183,7 @@
         <v>66</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7175,6 +7199,7 @@
       <c r="D6" s="14" t="n">
         <v>0.53125</v>
       </c>
+      <c r="E6" s="0"/>
       <c r="F6" s="15" t="n">
         <f aca="false">((HOUR(D6)-HOUR(C6))*60)+(MINUTE(D6)-MINUTE(C6))-E6</f>
         <v>165</v>
@@ -7183,12 +7208,12 @@
         <v>67</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="13" t="n">
-        <v>41937</v>
+        <v>41968</v>
       </c>
       <c r="B7" s="7" t="n">
         <v>10</v>
@@ -7199,6 +7224,7 @@
       <c r="D7" s="14" t="n">
         <v>0.614583333333333</v>
       </c>
+      <c r="E7" s="0"/>
       <c r="F7" s="15" t="n">
         <f aca="false">((HOUR(D7)-HOUR(C7))*60)+(MINUTE(D7)-MINUTE(C7))-E7</f>
         <v>105</v>
@@ -7207,12 +7233,12 @@
         <v>68</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="n">
-        <v>41938</v>
+        <v>41969</v>
       </c>
       <c r="B8" s="7" t="n">
         <v>10</v>
@@ -7223,6 +7249,7 @@
       <c r="D8" s="14" t="n">
         <v>0.690972222222222</v>
       </c>
+      <c r="E8" s="0"/>
       <c r="F8" s="15" t="n">
         <f aca="false">((HOUR(D8)-HOUR(C8))*60)+(MINUTE(D8)-MINUTE(C8))-E8</f>
         <v>110</v>
@@ -7231,12 +7258,12 @@
         <v>69</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="13" t="n">
-        <v>41939</v>
+        <v>41970</v>
       </c>
       <c r="B9" s="7" t="n">
         <v>10</v>
@@ -7247,6 +7274,7 @@
       <c r="D9" s="14" t="n">
         <v>0.506944444444444</v>
       </c>
+      <c r="E9" s="0"/>
       <c r="F9" s="15" t="n">
         <f aca="false">((HOUR(D9)-HOUR(C9))*60)+(MINUTE(D9)-MINUTE(C9))-E9</f>
         <v>240</v>
@@ -7255,7 +7283,61 @@
         <v>59</v>
       </c>
       <c r="H9" s="16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="13" t="n">
+        <v>41974</v>
+      </c>
+      <c r="B10" s="7" t="n">
+        <v>11</v>
+      </c>
+      <c r="C10" s="14" t="n">
+        <v>0.381944444444444</v>
+      </c>
+      <c r="D10" s="14" t="n">
+        <v>0.475694444444444</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="F10" s="15" t="n">
+        <f aca="false">((HOUR(D10)-HOUR(C10))*60)+(MINUTE(D10)-MINUTE(C10))-E10</f>
+        <v>120</v>
+      </c>
+      <c r="G10" s="7" t="n">
+        <v>75</v>
+      </c>
+      <c r="H10" s="16" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="13" t="n">
+        <v>41977</v>
+      </c>
+      <c r="B11" s="7" t="n">
+        <v>11</v>
+      </c>
+      <c r="C11" s="14" t="n">
+        <v>0.386805555555556</v>
+      </c>
+      <c r="D11" s="14" t="n">
+        <v>0.423611111111111</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="F11" s="15" t="n">
+        <f aca="false">((HOUR(D11)-HOUR(C11))*60)+(MINUTE(D11)-MINUTE(C11))-E11</f>
+        <v>43</v>
+      </c>
+      <c r="G11" s="7" t="n">
+        <v>78</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>